<commit_message>
fix the security bugs
</commit_message>
<xml_diff>
--- a/documentation/User Stories.xlsx
+++ b/documentation/User Stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinbai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinbai\Desktop\Capstone-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -615,7 +615,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -878,22 +878,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F12" s="13">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G12" s="13">
         <v>2</v>
@@ -901,22 +901,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" s="13">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G13" s="13">
         <v>2</v>
@@ -924,22 +924,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F14" s="13">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G14" s="13">
         <v>2</v>

</xml_diff>